<commit_message>
Rician bias 보정 전체
</commit_message>
<xml_diff>
--- a/SNR_by_Echo.xlsx
+++ b/SNR_by_Echo.xlsx
@@ -401,68 +401,68 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>6.319486618041992</v>
+        <v>1.886208295822144</v>
       </c>
       <c r="B2">
-        <v>11.99500179290771</v>
+        <v>9.377218246459961</v>
       </c>
       <c r="C2">
-        <v>5.675515174865723</v>
+        <v>7.491009712219238</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>3.385870456695557</v>
+        <v>-1.054936528205872</v>
       </c>
       <c r="B3">
-        <v>9.234843254089355</v>
+        <v>6.329257488250732</v>
       </c>
       <c r="C3">
-        <v>5.848972797393799</v>
+        <v>7.384193897247314</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>0.1748888194561005</v>
+        <v>-4.264941215515137</v>
       </c>
       <c r="B4">
-        <v>5.911576747894287</v>
+        <v>2.887811422348022</v>
       </c>
       <c r="C4">
-        <v>5.736688137054443</v>
+        <v>7.152752876281738</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>-3.104887008666992</v>
+        <v>-7.546406269073486</v>
       </c>
       <c r="B5">
-        <v>2.403767824172974</v>
+        <v>-0.6539157629013062</v>
       </c>
       <c r="C5">
-        <v>5.508654594421387</v>
+        <v>6.892490386962891</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>-6.120525360107422</v>
+        <v>-10.55385971069336</v>
       </c>
       <c r="B6">
-        <v>-1.004189491271973</v>
+        <v>-4.003417015075684</v>
       </c>
       <c r="C6">
-        <v>5.116335868835449</v>
+        <v>6.550442695617676</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>-8.592168807983398</v>
+        <v>-13.02655410766602</v>
       </c>
       <c r="B7">
-        <v>-4.269073963165283</v>
+        <v>-6.857790470123291</v>
       </c>
       <c r="C7">
-        <v>4.323094844818115</v>
+        <v>6.168763637542725</v>
       </c>
     </row>
   </sheetData>
@@ -491,68 +491,68 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>12.52652645111084</v>
+        <v>8.391603469848633</v>
       </c>
       <c r="B2">
-        <v>17.93169593811035</v>
+        <v>15.32101249694824</v>
       </c>
       <c r="C2">
-        <v>5.405169486999512</v>
+        <v>6.929409027099609</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>11.75560760498047</v>
+        <v>7.670703411102295</v>
       </c>
       <c r="B3">
-        <v>17.63250541687012</v>
+        <v>14.7795581817627</v>
       </c>
       <c r="C3">
-        <v>5.876897811889648</v>
+        <v>7.1088547706604</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>10.99514389038086</v>
+        <v>6.96019172668457</v>
       </c>
       <c r="B4">
-        <v>16.8945198059082</v>
+        <v>13.95021629333496</v>
       </c>
       <c r="C4">
-        <v>5.899375915527344</v>
+        <v>6.990024566650391</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>10.24566650390625</v>
+        <v>6.286073684692383</v>
       </c>
       <c r="B5">
-        <v>15.96136093139648</v>
+        <v>13.01476860046387</v>
       </c>
       <c r="C5">
-        <v>5.715694427490234</v>
+        <v>6.728694915771484</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>9.505977630615234</v>
+        <v>5.618660926818848</v>
       </c>
       <c r="B6">
-        <v>14.80568313598633</v>
+        <v>11.93073844909668</v>
       </c>
       <c r="C6">
-        <v>5.299705505371094</v>
+        <v>6.312077522277832</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>8.781160354614258</v>
+        <v>4.953777313232422</v>
       </c>
       <c r="B7">
-        <v>13.20557117462158</v>
+        <v>10.77796459197998</v>
       </c>
       <c r="C7">
-        <v>4.424410820007324</v>
+        <v>5.824187278747559</v>
       </c>
     </row>
   </sheetData>
@@ -581,68 +581,68 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>12.30920886993408</v>
+        <v>7.935194492340088</v>
       </c>
       <c r="B2">
-        <v>17.76426696777344</v>
+        <v>15.01033878326416</v>
       </c>
       <c r="C2">
-        <v>5.455058097839355</v>
+        <v>7.075144290924072</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>11.49683570861816</v>
+        <v>7.150395393371582</v>
       </c>
       <c r="B3">
-        <v>17.39969444274902</v>
+        <v>14.36503887176514</v>
       </c>
       <c r="C3">
-        <v>5.902858734130859</v>
+        <v>7.214643478393555</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>10.68100452423096</v>
+        <v>6.372131824493408</v>
       </c>
       <c r="B4">
-        <v>16.57991981506348</v>
+        <v>13.40629577636719</v>
       </c>
       <c r="C4">
-        <v>5.89891529083252</v>
+        <v>7.034163951873779</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>9.869684219360352</v>
+        <v>5.629256248474121</v>
       </c>
       <c r="B5">
-        <v>15.55800247192383</v>
+        <v>12.3375883102417</v>
       </c>
       <c r="C5">
-        <v>5.688318252563477</v>
+        <v>6.708332061767578</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>9.061206817626953</v>
+        <v>4.897980690002441</v>
       </c>
       <c r="B6">
-        <v>14.32855033874512</v>
+        <v>11.15977764129639</v>
       </c>
       <c r="C6">
-        <v>5.267343521118164</v>
+        <v>6.261796951293945</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>8.265759468078613</v>
+        <v>4.167629718780518</v>
       </c>
       <c r="B7">
-        <v>12.69919490814209</v>
+        <v>9.93265438079834</v>
       </c>
       <c r="C7">
-        <v>4.433435440063477</v>
+        <v>5.765024662017822</v>
       </c>
     </row>
   </sheetData>

</xml_diff>